<commit_message>
template file with changed names
</commit_message>
<xml_diff>
--- a/inst/extdata/config_pub_files.xlsx
+++ b/inst/extdata/config_pub_files.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/barbaramaria/surfdrive/Programming/OAmonitoring/config/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/barbaramaria/surfdrive/Programming/OAmonitor/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62A0AFC3-9A93-FE48-89DD-3F980182D3FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{067247F0-A7E9-AE4A-98A6-1F416C672E91}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="540" windowWidth="13080" windowHeight="17260" xr2:uid="{EC4569DB-D389-4344-A1CE-1A1B2B7F57C3}"/>
   </bookViews>
@@ -66,12 +66,6 @@
     <t>subject</t>
   </si>
   <si>
-    <t>mockdata_dighum_2018.csv</t>
-  </si>
-  <si>
-    <t>mockdata_niche_2018.tsv</t>
-  </si>
-  <si>
     <t>Other columns to include</t>
   </si>
   <si>
@@ -97,6 +91,12 @@
   </si>
   <si>
     <t>all</t>
+  </si>
+  <si>
+    <t>niches.tsv</t>
+  </si>
+  <si>
+    <t>digital_humanities.csv</t>
   </si>
 </sst>
 </file>
@@ -500,7 +500,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -531,10 +531,10 @@
         <v>7</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
@@ -544,13 +544,13 @@
     </row>
     <row r="3" spans="1:8" ht="29" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>19</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
@@ -592,11 +592,11 @@
     </row>
     <row r="6" spans="1:8" ht="29" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
@@ -622,7 +622,7 @@
     </row>
     <row r="8" spans="1:8" ht="29" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>10</v>
@@ -638,13 +638,13 @@
     </row>
     <row r="9" spans="1:8" ht="29" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="5"/>

</xml_diff>

<commit_message>
re-saved because possible corruption
</commit_message>
<xml_diff>
--- a/inst/extdata/config_pub_files.xlsx
+++ b/inst/extdata/config_pub_files.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/barbaramaria/surfdrive/Programming/OAmonitor/inst/extdata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vreed003\Dropbox\saved_repos_from_mac\OAmonitor\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{067247F0-A7E9-AE4A-98A6-1F416C672E91}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EE7C66BC-CFB2-4BC4-8DF2-E4A555CA8952}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="540" windowWidth="13080" windowHeight="17260" xr2:uid="{EC4569DB-D389-4344-A1CE-1A1B2B7F57C3}"/>
+    <workbookView xWindow="2955" yWindow="1560" windowWidth="20550" windowHeight="11835" xr2:uid="{EC4569DB-D389-4344-A1CE-1A1B2B7F57C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -503,14 +503,14 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.1640625" customWidth="1"/>
-    <col min="2" max="2" width="28.33203125" customWidth="1"/>
-    <col min="3" max="3" width="29.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.125" customWidth="1"/>
+    <col min="2" max="2" width="28.375" customWidth="1"/>
+    <col min="3" max="3" width="29.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="29.1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -526,7 +526,7 @@
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
     </row>
-    <row r="2" spans="1:8" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="29.1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -542,7 +542,7 @@
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="1:8" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="29.1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
@@ -558,7 +558,7 @@
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
     </row>
-    <row r="4" spans="1:8" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="29.1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -574,7 +574,7 @@
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
     </row>
-    <row r="5" spans="1:8" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="29.1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -590,7 +590,7 @@
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
     </row>
-    <row r="6" spans="1:8" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="29.1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>14</v>
       </c>
@@ -604,7 +604,7 @@
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
     </row>
-    <row r="7" spans="1:8" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="29.1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>1</v>
       </c>
@@ -620,7 +620,7 @@
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
     </row>
-    <row r="8" spans="1:8" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="29.1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>16</v>
       </c>
@@ -636,7 +636,7 @@
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
     </row>
-    <row r="9" spans="1:8" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="29.1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>11</v>
       </c>

</xml_diff>